<commit_message>
today's entry + adding raw data and obj summary
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Criz_sel_combination/Criz_sel_SRB_data.xlsx
+++ b/Raw_SRB_data/Criz_sel_combination/Criz_sel_SRB_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CxS 1" sheetId="1" r:id="rId1"/>
@@ -1392,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,7 +2150,7 @@
         <v>0.94833333333333336</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="C18:H18" si="0">AVERAGE(E9:E11)</f>
+        <f t="shared" ref="E18:H18" si="0">AVERAGE(E9:E11)</f>
         <v>0.69899999999999995</v>
       </c>
       <c r="F18">
@@ -2218,7 +2218,7 @@
         <v>0.8886666666666666</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:H20" si="2">AVERAGE(C12:C14)</f>
+        <f t="shared" ref="C20:G20" si="2">AVERAGE(C12:C14)</f>
         <v>0.51766666666666661</v>
       </c>
       <c r="D20">
@@ -2393,12 +2393,18 @@
       <c r="F25" s="1">
         <v>0.51766666666666661</v>
       </c>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1">
+        <f>F25/0.888667*100</f>
+        <v>58.252041165776006</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1">
         <v>0.45966666666666667</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="J25" s="1">
+        <f>I25/0.813*100</f>
+        <v>56.539565395653959</v>
+      </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2424,17 +2430,26 @@
       <c r="C26" s="1">
         <v>0.94833333333333336</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1">
+        <f t="shared" ref="D26:D30" si="3">C26/0.896*100</f>
+        <v>105.84077380952381</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1">
         <v>0.41</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1">
+        <f t="shared" ref="G26:G30" si="4">F26/0.888667*100</f>
+        <v>46.136516828013193</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1">
         <v>0.40233333333333327</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1">
+        <f t="shared" ref="J26:J30" si="5">I26/0.813*100</f>
+        <v>49.487494874948744</v>
+      </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2460,17 +2475,26 @@
       <c r="C27" s="1">
         <v>0.69899999999999995</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1">
+        <f t="shared" si="3"/>
+        <v>78.013392857142847</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1">
         <v>0.32333333333333331</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1">
+        <f t="shared" si="4"/>
+        <v>36.384082376563249</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1">
         <v>0.27966666666666667</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1">
+        <f t="shared" si="5"/>
+        <v>34.399343993439942</v>
+      </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2496,17 +2520,26 @@
       <c r="C28" s="1">
         <v>0.4423333333333333</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1">
+        <f t="shared" si="3"/>
+        <v>49.367559523809518</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1">
         <v>0.32500000000000001</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1">
+        <f t="shared" si="4"/>
+        <v>36.571629192937287</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1">
         <v>0.18899999999999997</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1">
+        <f t="shared" si="5"/>
+        <v>23.247232472324722</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2532,17 +2565,26 @@
       <c r="C29" s="1">
         <v>0.26499999999999996</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1">
+        <f t="shared" si="3"/>
+        <v>29.575892857142851</v>
+      </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1">
         <v>0.253</v>
       </c>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1">
+        <f t="shared" si="4"/>
+        <v>28.469606725578871</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1">
         <v>0.13333333333333333</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1">
+        <f t="shared" si="5"/>
+        <v>16.400164001640015</v>
+      </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2568,17 +2610,26 @@
       <c r="C30" s="1">
         <v>0.21299999999999999</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1">
+        <f t="shared" si="3"/>
+        <v>23.772321428571427</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1">
         <v>0.18000000000000002</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1">
+        <f t="shared" si="4"/>
+        <v>20.255056168396038</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1">
         <v>8.7333333333333332E-2</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="1">
+        <f t="shared" si="5"/>
+        <v>10.742107421074211</v>
+      </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2802,7 +2853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating raw data + last week's entries
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Criz_sel_combination/Criz_sel_SRB_data.xlsx
+++ b/Raw_SRB_data/Criz_sel_combination/Criz_sel_SRB_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CxS 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Crizotinib</t>
   </si>
@@ -1392,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24:J30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,46 +2851,937 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="B8">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C8">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D8">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F8">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.05</v>
+      </c>
+      <c r="H8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J8">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="L8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="N8">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="O8">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="P8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="Q8">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="R8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="S8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="T8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="U8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="V8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="W8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="X8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="Y8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.444</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1.3720000000000001</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.3029999999999999</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1.486</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="I9">
+        <v>5.5E-2</v>
+      </c>
+      <c r="J9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="K9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="L9">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="N9">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1.6679999999999999</v>
+      </c>
+      <c r="P9" s="4">
+        <v>1.4810000000000001</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="T9" s="4">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="V9">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="W9">
+        <v>0.05</v>
+      </c>
+      <c r="X9">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="Y9">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1.569</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.21</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1.2310000000000001</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="I10">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="J10">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K10">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="L10">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="N10">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1.3240000000000001</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="S10" s="4">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="T10" s="4">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="U10" s="4">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="V10">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="W10">
+        <v>0.05</v>
+      </c>
+      <c r="X10">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="Y10">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.661</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.7809999999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.6850000000000001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="I11">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="J11">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K11">
+        <v>0.06</v>
+      </c>
+      <c r="L11">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="N11">
+        <v>4.7E-2</v>
+      </c>
+      <c r="O11" s="4">
+        <v>1.774</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1.415</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="S11" s="4">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="T11" s="4">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="U11" s="4">
+        <v>0.245</v>
+      </c>
+      <c r="V11">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="W11">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="X11">
+        <v>5.5E-2</v>
+      </c>
+      <c r="Y11">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.8919999999999999</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.1459999999999999</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.3380000000000001</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="I12">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="J12">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K12">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="L12">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="N12">
+        <v>0.05</v>
+      </c>
+      <c r="O12">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="P12">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="Q12">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="R12">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="S12">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="T12">
+        <v>5.5E-2</v>
+      </c>
+      <c r="U12">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="V12">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="W12">
+        <v>4.7E-2</v>
+      </c>
+      <c r="X12">
+        <v>5.5E-2</v>
+      </c>
+      <c r="Y12">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1.579</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.143</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="I13">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.06</v>
+      </c>
+      <c r="K13">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="L13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="N13">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="O13">
+        <v>5.5E-2</v>
+      </c>
+      <c r="P13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="Q13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="R13">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="S13">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="T13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="U13">
+        <v>5.5E-2</v>
+      </c>
+      <c r="V13">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="W13">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="X13">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="Y13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.605</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.1140000000000001</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="I14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J14">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="K14">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="L14">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="N14">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="O14">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="P14">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="Q14">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="R14">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="S14">
+        <v>6.3E-2</v>
+      </c>
+      <c r="T14">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="U14">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="V14">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="W14">
+        <v>0.06</v>
+      </c>
+      <c r="X14">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="Y14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="B15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C15">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E15">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F15">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I15">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="J15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L15">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="N15">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="O15">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="P15">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="Q15">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="R15">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="S15">
+        <v>0.05</v>
+      </c>
+      <c r="T15">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="U15">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="V15">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="W15">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="X15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="Y15">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <f>AVERAGE(B9:B11)</f>
+        <v>1.5579999999999998</v>
+      </c>
+      <c r="C18">
+        <f>AVERAGE(C9:C11)</f>
+        <v>1.4543333333333333</v>
+      </c>
+      <c r="D18">
+        <f>AVERAGE(D9:D11)</f>
+        <v>1.3626666666666667</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:H18" si="0">AVERAGE(E9:E11)</f>
+        <v>1.2783333333333333</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.81866666666666665</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0.49266666666666675</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0.26766666666666666</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18">
+        <f>AVERAGE(O9:O11)</f>
+        <v>1.5783333333333331</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18:U18" si="1">AVERAGE(P9:P11)</f>
+        <v>1.406666666666667</v>
+      </c>
+      <c r="Q18">
+        <f>AVERAGE(Q9:Q11)</f>
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>0.78433333333333322</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="1"/>
+        <v>0.53433333333333333</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="1"/>
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="1"/>
+        <v>0.20433333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <f>AVERAGE(B12:B14)</f>
+        <v>1.6920000000000002</v>
+      </c>
+      <c r="C20">
+        <f>AVERAGE(C12:C14)</f>
+        <v>1.0570000000000002</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="C20:G20" si="2">AVERAGE(D12:D14)</f>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>0.86266666666666669</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>0.67533333333333323</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>0.63733333333333331</v>
+      </c>
+      <c r="H20">
+        <f>AVERAGE(H12:H14)</f>
+        <v>0.40500000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="F23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="I23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1.5579999999999998</v>
+      </c>
+      <c r="D24">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>1.6920000000000002</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+      <c r="I24">
+        <v>1.5783333333333331</v>
+      </c>
+      <c r="J24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.1</v>
+      </c>
+      <c r="C25">
+        <v>1.4543333333333333</v>
+      </c>
+      <c r="D25">
+        <f>C25/1.558*100</f>
+        <v>93.346170303808293</v>
+      </c>
+      <c r="F25">
+        <v>1.0570000000000002</v>
+      </c>
+      <c r="G25">
+        <f>F25/1.692*100</f>
+        <v>62.470449172576849</v>
+      </c>
+      <c r="I25">
+        <v>1.406666666666667</v>
+      </c>
+      <c r="J25">
+        <f>I25/1.578333*100</f>
+        <v>89.123566868757536</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.25</v>
+      </c>
+      <c r="C26">
+        <v>1.3626666666666667</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:D30" si="3">C26/1.558*100</f>
+        <v>87.462558836114681</v>
+      </c>
+      <c r="F26">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G30" si="4">F26/1.692*100</f>
+        <v>64.420803782505914</v>
+      </c>
+      <c r="I26">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ref="J26:J30" si="5">I26/1.578333*100</f>
+        <v>54.677941853841993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.5</v>
+      </c>
+      <c r="C27">
+        <v>1.2783333333333333</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="3"/>
+        <v>82.049636285836542</v>
+      </c>
+      <c r="F27">
+        <v>0.86266666666666669</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>50.985027580772268</v>
+      </c>
+      <c r="I27">
+        <v>0.78433333333333322</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>49.693780294356969</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.81866666666666665</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>52.545999144201957</v>
+      </c>
+      <c r="F28">
+        <v>0.67533333333333323</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>39.913317572892041</v>
+      </c>
+      <c r="I28">
+        <v>0.53433333333333333</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>33.854283812942725</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2.5</v>
+      </c>
+      <c r="C29">
+        <v>0.49266666666666675</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>31.621737270004285</v>
+      </c>
+      <c r="F29">
+        <v>0.63733333333333331</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="4"/>
+        <v>37.667454688731283</v>
+      </c>
+      <c r="I29">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>15.332632594008997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>0.26766666666666666</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>17.180145485665381</v>
+      </c>
+      <c r="F30">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="4"/>
+        <v>23.936170212765958</v>
+      </c>
+      <c r="I30">
+        <v>0.20433333333333334</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>12.946148457475914</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>